<commit_message>
Multiple Scenario testcases execution added and Switch case removed from test executor
</commit_message>
<xml_diff>
--- a/KeywordDrivenFramework/src/main/resources/test_data.xlsx
+++ b/KeywordDrivenFramework/src/main/resources/test_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tejas\eclipse-workspace\KeywordDrivenFramework\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tejas\git\Automation\KeywordDrivenFramework\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A59CD92-55AF-4F18-B11F-ABEB53611D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF80825-89A2-42B8-AEAF-AC50D3657ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7035" yWindow="2400" windowWidth="21600" windowHeight="11295" xr2:uid="{047D0D55-4AA9-43C2-9B58-13282705AF08}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="20">
   <si>
     <t>Keyword</t>
   </si>
@@ -58,41 +58,50 @@
     <t>verifyText</t>
   </si>
   <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/auth/login</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>//*[@placeholder='Password']</t>
+  </si>
+  <si>
+    <t>//button</t>
+  </si>
+  <si>
+    <t>//span[text()='Dashboard']</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>//*[@placeholder='Username']</t>
+  </si>
+  <si>
+    <t>TestCaseID</t>
+  </si>
+  <si>
+    <t>TC_001</t>
+  </si>
+  <si>
+    <t>TC_002</t>
+  </si>
+  <si>
+    <t>openBrowser</t>
+  </si>
+  <si>
     <t>closeBrowser</t>
-  </si>
-  <si>
-    <t>https://opensource-demo.orangehrmlive.com/web/index.php/auth/login</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>//*[@placeholder='Password']</t>
-  </si>
-  <si>
-    <t>//button</t>
-  </si>
-  <si>
-    <t>//span[text()='Dashboard']</t>
-  </si>
-  <si>
-    <t>Dashboard</t>
-  </si>
-  <si>
-    <t>//*[@placeholder='Username']</t>
-  </si>
-  <si>
-    <t>Welcome</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,8 +125,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,6 +142,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -159,7 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -170,6 +191,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -485,91 +515,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9146C13-38E6-4E83-ADDE-880847686D85}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
-    <col min="3" max="3" width="70" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{DBF52563-3547-4E51-B374-E2DBE0B28718}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{DBF52563-3547-4E51-B374-E2DBE0B28718}"/>
+    <hyperlink ref="D10" r:id="rId2" xr:uid="{3A0BB3F0-56C3-4F30-A342-C1D4C4467E7E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -577,10 +726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3F96EB-7EB5-41EB-B02D-0C2F19E64A2C}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +756,7 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -615,10 +764,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -626,10 +775,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -637,7 +786,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -646,18 +795,11 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>